<commit_message>
MODIFY Group Fund.xlsx Add a ID Field
</commit_message>
<xml_diff>
--- a/Group Fund.xlsx
+++ b/Group Fund.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="8445"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>status</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Thi Nguyen</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -53,7 +56,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -375,59 +378,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.25" customWidth="1"/>
+    <col min="3" max="3" width="10.375" customWidth="1"/>
+    <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>5000</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>40430</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>5000</v>
       </c>
     </row>
@@ -442,7 +451,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -454,7 +463,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MODIFY /trunk/Minutes/2010_09_30.docx correct some English mistakes MODIFY /trunk/Group Fund.xlsx         update Group Fund information ADD    /branches/Thi/Constructing Attack Scenarios through Correlation of Intrusion Alerts.pdf  add Peng Ning's paper about Alert Correlation ADD    /branches/Thi/Constructing Attack Scenarios through Correlation of Intrusion Alerts.docx report about this paper
</commit_message>
<xml_diff>
--- a/Group Fund.xlsx
+++ b/Group Fund.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>status</t>
   </si>
@@ -24,9 +24,6 @@
     <t>sum</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -39,13 +36,22 @@
     <t>late for meeting</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>Thi Nguyen</t>
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Waiting</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Tan Nguyen</t>
+  </si>
+  <si>
+    <t>amount (VND)</t>
   </si>
 </sst>
 </file>
@@ -56,17 +62,23 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,9 +93,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,34 +401,35 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.25" customWidth="1"/>
-    <col min="3" max="3" width="10.375" customWidth="1"/>
-    <col min="4" max="4" width="12.75" customWidth="1"/>
-    <col min="5" max="5" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -420,16 +441,56 @@
         <v>5000</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>40430</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>40444</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
-        <v>40430</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>15000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3">
+        <v>40444</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -437,7 +498,8 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>5000</v>
+        <f>SUM(B2:B11)</f>
+        <v>30000</v>
       </c>
     </row>
   </sheetData>
@@ -451,7 +513,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -463,7 +525,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modify trunk/Group Fund.xlsx update fund
</commit_message>
<xml_diff>
--- a/Group Fund.xlsx
+++ b/Group Fund.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="8445"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>status</t>
   </si>
@@ -401,7 +401,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -493,13 +493,33 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>10000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3">
+        <v>40465</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13">
         <f>SUM(B2:B11)</f>
-        <v>30000</v>
+        <v>40000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD Minutes/2010_12_5.docx ADD Group Rules.docx MODIFY Group Fund.xlsx
</commit_message>
<xml_diff>
--- a/Group Fund.xlsx
+++ b/Group Fund.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="8445"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>status</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>amount (VND)</t>
+  </si>
+  <si>
+    <t>Mr Tan has the responsibility to get and save the group fund.</t>
   </si>
 </sst>
 </file>
@@ -67,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -77,6 +80,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -93,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -103,6 +112,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -398,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -413,7 +425,7 @@
     <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1">
+    <row r="1" spans="1:15" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -432,8 +444,18 @@
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -452,8 +474,16 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -472,8 +502,16 @@
       <c r="F3" t="s">
         <v>8</v>
       </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -493,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -513,7 +551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:15">
       <c r="B13" t="s">
         <v>1</v>
       </c>
@@ -523,7 +561,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:O3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ADD trunk/Minutes/2010_12_20.docx add new minute MODIFY trunk/Group Fund.xlsx update group fund
</commit_message>
<xml_diff>
--- a/Group Fund.xlsx
+++ b/Group Fund.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="8445"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>status</t>
   </si>
@@ -55,6 +55,27 @@
   </si>
   <si>
     <t>Mr Tan has the responsibility to get and save the group fund.</t>
+  </si>
+  <si>
+    <t>Thang Duong</t>
+  </si>
+  <si>
+    <t>…..</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Kim Hoang</t>
+  </si>
+  <si>
+    <t>no submit</t>
+  </si>
+  <si>
+    <t>rule 19</t>
+  </si>
+  <si>
+    <t>Thang Le</t>
   </si>
 </sst>
 </file>
@@ -410,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -551,13 +572,193 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>10000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>10000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>10000</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>10000</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3">
+        <v>40433</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>10000</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>40433</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10000</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3">
+        <v>40532</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>10000</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3">
+        <v>40532</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="13" spans="1:15">
-      <c r="B13" t="s">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>10000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3">
+        <v>40532</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>10000</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3">
+        <v>40532</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C13">
-        <f>SUM(B2:B11)</f>
-        <v>40000</v>
+      <c r="C20">
+        <f>SUM(B2:B16)</f>
+        <v>130000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>